<commit_message>
13th July code Registeration module
</commit_message>
<xml_diff>
--- a/Extra/TestCases.xlsx
+++ b/Extra/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
   <si>
     <t>Prepared By:</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>TC_ID9</t>
+  </si>
+  <si>
+    <t>user_Registeration()</t>
+  </si>
+  <si>
+    <t>user_Registeration_Validations()</t>
   </si>
   <si>
     <t>PASS</t>
@@ -189,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="66" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,10 +279,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -328,12 +334,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <sz val="15.0"/>
       <b val="true"/>
       <color indexed="10"/>
@@ -343,6 +343,258 @@
       <sz val="11.0"/>
       <b val="true"/>
       <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -433,7 +685,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -484,32 +736,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,11 +751,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -536,6 +788,47 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -844,7 +1137,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I6" sqref="I6:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,42 +1975,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1773,60 +2066,60 @@
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="31" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s" s="51">
-        <v>54</v>
-      </c>
-      <c r="J6" s="26"/>
+      <c r="I6" t="s" s="85">
+        <v>57</v>
+      </c>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="28"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="14" t="s">
         <v>23</v>
       </c>
@@ -1836,8 +2129,8 @@
       <c r="H8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I8" t="s" s="47">
-        <v>54</v>
+      <c r="I8" t="s" s="86">
+        <v>57</v>
       </c>
       <c r="J8" s="12"/>
     </row>
@@ -1845,8 +2138,8 @@
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="35" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -1864,16 +2157,16 @@
       <c r="H9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s" s="48">
-        <v>54</v>
+      <c r="I9" t="s" s="87">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
@@ -1889,8 +2182,8 @@
       <c r="H10" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I10" t="s" s="49">
-        <v>54</v>
+      <c r="I10" t="s" s="88">
+        <v>57</v>
       </c>
       <c r="J10" s="12"/>
     </row>
@@ -1898,50 +2191,50 @@
       <c r="A11" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="35" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I11" t="s" s="40">
-        <v>54</v>
+      <c r="I11" t="s" s="89">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="28"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="36"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1957,8 +2250,8 @@
       <c r="H13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I13" t="s" s="41">
-        <v>54</v>
+      <c r="I13" t="s" s="90">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1971,8 +2264,14 @@
       <c r="D14" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="F14" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="H14" s="19" t="s">
         <v>46</v>
+      </c>
+      <c r="I14" t="s" s="91">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1982,15 +2281,29 @@
       <c r="D15" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="F15" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="G15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>48</v>
+      </c>
+      <c r="I15" t="s" s="92">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:J3"/>
     <mergeCell ref="C6:C8"/>
@@ -1999,14 +2312,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
improve resume Link Verification
</commit_message>
<xml_diff>
--- a/Extra/TestCases.xlsx
+++ b/Extra/TestCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
   <si>
     <t>Prepared By:</t>
   </si>
@@ -226,10 +226,79 @@
     <t>18,8</t>
   </si>
   <si>
-    <t>Sunil,anil33@mailinator.com,f00bar12,f00bar12,9910881849</t>
+    <t>To Verify Click on  magic resume india</t>
+  </si>
+  <si>
+    <t>19,8</t>
+  </si>
+  <si>
+    <t>To Verify Click on  magic resume international</t>
+  </si>
+  <si>
+    <t>Click_MRI()</t>
+  </si>
+  <si>
+    <t>Click_MR_International()</t>
+  </si>
+  <si>
+    <t>20,8</t>
+  </si>
+  <si>
+    <t>To verify clicking on Resume Critique</t>
+  </si>
+  <si>
+    <t>click_ResumeCritique()</t>
+  </si>
+  <si>
+    <t>21,8</t>
+  </si>
+  <si>
+    <t>To Verify Clicking on Social Profiler</t>
+  </si>
+  <si>
+    <t>To Verify clicking on Visual Resume Premium</t>
+  </si>
+  <si>
+    <t>To verify clicking on View all services</t>
+  </si>
+  <si>
+    <t>To verify clicking on View sample resume</t>
+  </si>
+  <si>
+    <t>click_socialprofiler()</t>
+  </si>
+  <si>
+    <t>click_visual_resume_premium()</t>
+  </si>
+  <si>
+    <t>click_view_all_services()</t>
+  </si>
+  <si>
+    <t>click_view_sample_resume()</t>
+  </si>
+  <si>
+    <t>22,8</t>
+  </si>
+  <si>
+    <t>23,8</t>
+  </si>
+  <si>
+    <t>24,8</t>
+  </si>
+  <si>
+    <t>25,8</t>
+  </si>
+  <si>
+    <t>Sunil,anil34@mailinator.com,f00bar12,f00bar12,9910881849</t>
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Login and Registeration</t>
   </si>
 </sst>
 </file>
@@ -237,7 +306,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,13 +355,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -482,93 +544,93 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
       <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
       <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
       <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
       <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
       <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="15.0"/>
       <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="17"/>
+      <color indexed="10"/>
     </font>
   </fonts>
   <fills count="26">
@@ -875,54 +937,54 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -973,12 +1035,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -986,6 +1047,12 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,7 +1062,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,23 +1085,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1 2" xfId="3"/>
@@ -1383,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I6:I19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,42 +2290,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -2315,60 +2381,60 @@
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="50" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s" s="47">
-        <v>71</v>
-      </c>
-      <c r="J6" s="33"/>
+      <c r="I6" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="37"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="44"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="35"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="42"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="14" t="s">
         <v>23</v>
       </c>
@@ -2378,8 +2444,8 @@
       <c r="H8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I8" t="s" s="48">
-        <v>71</v>
+      <c r="I8" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="J8" s="12"/>
     </row>
@@ -2387,8 +2453,8 @@
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="40" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -2406,16 +2472,16 @@
       <c r="H9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s" s="49">
-        <v>71</v>
+      <c r="I9" s="24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="17" t="s">
         <v>26</v>
       </c>
@@ -2431,8 +2497,8 @@
       <c r="H10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I10" t="s" s="50">
-        <v>71</v>
+      <c r="I10" s="25" t="s">
+        <v>92</v>
       </c>
       <c r="J10" s="12"/>
     </row>
@@ -2440,50 +2506,50 @@
       <c r="A11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="41"/>
+      <c r="C11" s="40" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="I11" t="s" s="51">
-        <v>71</v>
+      <c r="I11" s="43" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="37"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="44"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2499,15 +2565,18 @@
       <c r="H13" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="I13" t="s" s="52">
-        <v>71</v>
+      <c r="I13" s="26" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="B14" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="40" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -2519,12 +2588,13 @@
       <c r="H14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I14" t="s" s="53">
-        <v>71</v>
+      <c r="I14" s="27" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="34"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="5" t="s">
         <v>40</v>
       </c>
@@ -2534,18 +2604,19 @@
       <c r="F15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>70</v>
+      <c r="G15" s="55" t="s">
+        <v>91</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I15" t="s" s="54">
-        <v>71</v>
+      <c r="I15" s="28" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="35"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="5" t="s">
         <v>53</v>
       </c>
@@ -2561,11 +2632,12 @@
       <c r="H16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="I16" t="s" s="55">
-        <v>71</v>
+      <c r="I16" s="29" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="54"/>
       <c r="C17" s="7" t="s">
         <v>56</v>
       </c>
@@ -2584,11 +2656,12 @@
       <c r="H17" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="I17" t="s" s="57">
-        <v>71</v>
+      <c r="I17" s="30" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="46"/>
       <c r="C18" s="7" t="s">
         <v>61</v>
       </c>
@@ -2607,12 +2680,15 @@
       <c r="H18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="I18" t="s" s="58">
-        <v>71</v>
+      <c r="I18" s="31" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="40" t="s">
         <v>66</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2624,18 +2700,175 @@
       <c r="F19" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="G19" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="H19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="I19" t="s" s="59">
+      <c r="I19" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>71</v>
       </c>
+      <c r="I20" t="s" s="56">
+        <v>93</v>
+      </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="22"/>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" t="s" s="57">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I22" t="s" s="58">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" t="s" s="59">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" t="s" s="60">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" t="s" s="61">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B26"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:J3"/>
     <mergeCell ref="C6:C8"/>

</xml_diff>